<commit_message>
Zoho library updated, multiple record mandatory field checking added
</commit_message>
<xml_diff>
--- a/uploads/my contacts.xlsx
+++ b/uploads/my contacts.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3252" yWindow="228" windowWidth="19320" windowHeight="11016" tabRatio="769"/>
+    <workbookView xWindow="3255" yWindow="225" windowWidth="19320" windowHeight="11010" tabRatio="769"/>
   </bookViews>
   <sheets>
     <sheet name="Registrations 12.10" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3154" uniqueCount="1777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3153" uniqueCount="1776">
   <si>
     <t>First</t>
   </si>
@@ -5233,9 +5233,6 @@
   </si>
   <si>
     <t>Anthony</t>
-  </si>
-  <si>
-    <t>DeNucci</t>
   </si>
   <si>
     <t>VP Information Services</t>
@@ -5355,8 +5352,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5545,7 +5542,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -5580,7 +5576,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5756,28 +5751,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I417"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I150" sqref="I150"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.44140625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="29.44140625" style="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="29.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5806,7 +5801,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>291</v>
       </c>
@@ -5835,15 +5830,12 @@
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>1737</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1738</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1739</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>294</v>
@@ -5855,10 +5847,10 @@
         <v>18</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1740</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
@@ -5887,7 +5879,7 @@
         <v>1464</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>1465</v>
       </c>
@@ -5916,7 +5908,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
@@ -5930,10 +5922,10 @@
         <v>1700</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>18</v>
@@ -5942,10 +5934,10 @@
         <v>8052</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>1585</v>
       </c>
@@ -5959,7 +5951,7 @@
         <v>1586</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>1652</v>
@@ -5971,7 +5963,7 @@
         <v>7631</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>1278</v>
       </c>
@@ -6000,7 +5992,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>1237</v>
       </c>
@@ -6029,7 +6021,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>1376</v>
       </c>
@@ -6058,7 +6050,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>1647</v>
       </c>
@@ -6087,7 +6079,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>1455</v>
       </c>
@@ -6116,7 +6108,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>537</v>
       </c>
@@ -6145,7 +6137,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>512</v>
       </c>
@@ -6174,7 +6166,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>1533</v>
       </c>
@@ -6203,7 +6195,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>843</v>
       </c>
@@ -6229,7 +6221,7 @@
         <v>7860</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -6258,7 +6250,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>148</v>
       </c>
@@ -6287,7 +6279,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>703</v>
       </c>
@@ -6313,7 +6305,7 @@
         <v>8540</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>1328</v>
       </c>
@@ -6339,7 +6331,7 @@
         <v>8540</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>1331</v>
       </c>
@@ -6368,7 +6360,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="1" t="s">
         <v>720</v>
       </c>
@@ -6397,7 +6389,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="1" t="s">
         <v>719</v>
       </c>
@@ -6426,7 +6418,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="1" t="s">
         <v>524</v>
       </c>
@@ -6440,10 +6432,10 @@
         <v>1697</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>1772</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="1" t="s">
         <v>1725</v>
       </c>
@@ -6472,7 +6464,7 @@
         <v>1728</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="1" t="s">
         <v>549</v>
       </c>
@@ -6501,7 +6493,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="1" t="s">
         <v>545</v>
       </c>
@@ -6530,7 +6522,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="1" t="s">
         <v>1171</v>
       </c>
@@ -6559,7 +6551,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="1" t="s">
         <v>483</v>
       </c>
@@ -6582,7 +6574,7 @@
         <v>7503</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="1" t="s">
         <v>879</v>
       </c>
@@ -6608,7 +6600,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="1" t="s">
         <v>311</v>
       </c>
@@ -6631,7 +6623,7 @@
         <v>7503</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="1" t="s">
         <v>134</v>
       </c>
@@ -6660,7 +6652,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
         <v>1084</v>
       </c>
@@ -6683,7 +6675,7 @@
         <v>7666</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
         <v>103</v>
       </c>
@@ -6712,7 +6704,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
         <v>312</v>
       </c>
@@ -6741,7 +6733,7 @@
         <v>1517</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
         <v>444</v>
       </c>
@@ -6770,7 +6762,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" s="1" t="s">
         <v>1049</v>
       </c>
@@ -6796,7 +6788,7 @@
         <v>8901</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
         <v>312</v>
       </c>
@@ -6825,7 +6817,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
         <v>325</v>
       </c>
@@ -6854,7 +6846,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
         <v>96</v>
       </c>
@@ -6883,7 +6875,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
         <v>1136</v>
       </c>
@@ -6912,7 +6904,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
         <v>20</v>
       </c>
@@ -6941,7 +6933,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
         <v>363</v>
       </c>
@@ -6970,7 +6962,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
         <v>243</v>
       </c>
@@ -6999,7 +6991,7 @@
         <v>1668</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
         <v>261</v>
       </c>
@@ -7028,7 +7020,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
         <v>1127</v>
       </c>
@@ -7051,7 +7043,7 @@
         <v>8401</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
         <v>341</v>
       </c>
@@ -7074,7 +7066,7 @@
         <v>8401</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
         <v>381</v>
       </c>
@@ -7103,7 +7095,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" s="1" t="s">
         <v>401</v>
       </c>
@@ -7132,7 +7124,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" s="1" t="s">
         <v>41</v>
       </c>
@@ -7161,7 +7153,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="A51" s="1" t="s">
         <v>408</v>
       </c>
@@ -7190,7 +7182,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9">
       <c r="A52" s="1" t="s">
         <v>434</v>
       </c>
@@ -7219,7 +7211,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" s="1" t="s">
         <v>201</v>
       </c>
@@ -7248,7 +7240,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="A54" s="1" t="s">
         <v>506</v>
       </c>
@@ -7277,7 +7269,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9">
       <c r="A55" s="1" t="s">
         <v>1143</v>
       </c>
@@ -7306,7 +7298,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="A56" s="1" t="s">
         <v>117</v>
       </c>
@@ -7335,7 +7327,7 @@
         <v>1724</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="A57" s="1" t="s">
         <v>549</v>
       </c>
@@ -7364,7 +7356,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">
         <v>570</v>
       </c>
@@ -7393,7 +7385,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9">
       <c r="A59" s="1" t="s">
         <v>20</v>
       </c>
@@ -7422,7 +7414,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9">
       <c r="A60" s="1" t="s">
         <v>69</v>
       </c>
@@ -7451,7 +7443,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9">
       <c r="A61" s="1" t="s">
         <v>25</v>
       </c>
@@ -7480,7 +7472,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9">
       <c r="A62" s="1" t="s">
         <v>248</v>
       </c>
@@ -7509,7 +7501,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9">
       <c r="A63" s="1" t="s">
         <v>243</v>
       </c>
@@ -7538,7 +7530,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9">
       <c r="A64" s="1" t="s">
         <v>32</v>
       </c>
@@ -7567,7 +7559,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9">
       <c r="A65" s="1" t="s">
         <v>1159</v>
       </c>
@@ -7581,7 +7573,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9">
       <c r="A66" s="1" t="s">
         <v>584</v>
       </c>
@@ -7610,7 +7602,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9">
       <c r="A67" s="1" t="s">
         <v>1024</v>
       </c>
@@ -7639,7 +7631,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9">
       <c r="A68" s="1" t="s">
         <v>103</v>
       </c>
@@ -7668,7 +7660,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9">
       <c r="A69" s="1" t="s">
         <v>341</v>
       </c>
@@ -7697,7 +7689,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9">
       <c r="A70" s="1" t="s">
         <v>387</v>
       </c>
@@ -7726,7 +7718,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9">
       <c r="A71" s="1" t="s">
         <v>32</v>
       </c>
@@ -7755,7 +7747,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9">
       <c r="A72" s="1" t="s">
         <v>526</v>
       </c>
@@ -7784,7 +7776,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9">
       <c r="A73" s="1" t="s">
         <v>420</v>
       </c>
@@ -7813,7 +7805,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9">
       <c r="A74" s="1" t="s">
         <v>1162</v>
       </c>
@@ -7842,7 +7834,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9">
       <c r="A75" s="1" t="s">
         <v>103</v>
       </c>
@@ -7871,7 +7863,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9">
       <c r="A76" s="1" t="s">
         <v>288</v>
       </c>
@@ -7897,7 +7889,7 @@
         <v>8007</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9">
       <c r="A77" s="1" t="s">
         <v>32</v>
       </c>
@@ -7926,7 +7918,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9">
       <c r="A78" s="1" t="s">
         <v>140</v>
       </c>
@@ -7955,7 +7947,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9">
       <c r="A79" s="1" t="s">
         <v>1357</v>
       </c>
@@ -7984,7 +7976,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9">
       <c r="A80" s="1" t="s">
         <v>96</v>
       </c>
@@ -8013,7 +8005,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9">
       <c r="A81" s="1" t="s">
         <v>1097</v>
       </c>
@@ -8030,7 +8022,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9">
       <c r="A82" s="1" t="s">
         <v>168</v>
       </c>
@@ -8059,7 +8051,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9">
       <c r="A83" s="1" t="s">
         <v>20</v>
       </c>
@@ -8088,7 +8080,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9">
       <c r="A84" s="1" t="s">
         <v>387</v>
       </c>
@@ -8117,7 +8109,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9">
       <c r="A85" s="1" t="s">
         <v>134</v>
       </c>
@@ -8146,7 +8138,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9">
       <c r="A86" s="1" t="s">
         <v>1370</v>
       </c>
@@ -8175,7 +8167,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9">
       <c r="A87" s="1" t="s">
         <v>47</v>
       </c>
@@ -8204,7 +8196,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9">
       <c r="A88" s="1" t="s">
         <v>54</v>
       </c>
@@ -8233,7 +8225,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9">
       <c r="A89" s="1" t="s">
         <v>51</v>
       </c>
@@ -8262,7 +8254,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9">
       <c r="A90" s="1" t="s">
         <v>128</v>
       </c>
@@ -8291,7 +8283,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9">
       <c r="A91" s="1" t="s">
         <v>47</v>
       </c>
@@ -8320,7 +8312,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9">
       <c r="A92" s="1" t="s">
         <v>1016</v>
       </c>
@@ -8349,7 +8341,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9">
       <c r="A93" s="1" t="s">
         <v>1491</v>
       </c>
@@ -8378,7 +8370,7 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9">
       <c r="A94" s="1" t="s">
         <v>564</v>
       </c>
@@ -8407,7 +8399,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9">
       <c r="A95" s="1" t="s">
         <v>140</v>
       </c>
@@ -8436,7 +8428,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9">
       <c r="A96" s="1" t="s">
         <v>524</v>
       </c>
@@ -8465,7 +8457,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9">
       <c r="A97" s="1" t="s">
         <v>1663</v>
       </c>
@@ -8491,7 +8483,7 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9">
       <c r="A98" s="1" t="s">
         <v>1657</v>
       </c>
@@ -8517,7 +8509,7 @@
         <v>1659</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9">
       <c r="A99" s="1" t="s">
         <v>524</v>
       </c>
@@ -8543,7 +8535,7 @@
         <v>1661</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9">
       <c r="A100" s="1" t="s">
         <v>134</v>
       </c>
@@ -8572,7 +8564,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9">
       <c r="A101" s="1" t="s">
         <v>285</v>
       </c>
@@ -8601,7 +8593,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9">
       <c r="A102" s="1" t="s">
         <v>1370</v>
       </c>
@@ -8630,7 +8622,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9">
       <c r="A103" s="1" t="s">
         <v>1418</v>
       </c>
@@ -8659,7 +8651,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9">
       <c r="A104" s="1" t="s">
         <v>20</v>
       </c>
@@ -8688,7 +8680,7 @@
         <v>1662</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9">
       <c r="A105" s="1" t="s">
         <v>549</v>
       </c>
@@ -8717,7 +8709,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9">
       <c r="A106" s="1" t="s">
         <v>7</v>
       </c>
@@ -8746,7 +8738,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9">
       <c r="A107" s="1" t="s">
         <v>54</v>
       </c>
@@ -8775,7 +8767,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9">
       <c r="A108" s="1" t="s">
         <v>975</v>
       </c>
@@ -8804,7 +8796,7 @@
         <v>1559</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9">
       <c r="A109" s="1" t="s">
         <v>622</v>
       </c>
@@ -8830,7 +8822,7 @@
         <v>8513</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9">
       <c r="A110" s="1" t="s">
         <v>208</v>
       </c>
@@ -8856,7 +8848,7 @@
         <v>8513</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9">
       <c r="A111" s="1" t="s">
         <v>624</v>
       </c>
@@ -8882,7 +8874,7 @@
         <v>8513</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9">
       <c r="A112" s="1" t="s">
         <v>7</v>
       </c>
@@ -8911,7 +8903,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9">
       <c r="A113" s="1" t="s">
         <v>526</v>
       </c>
@@ -8940,7 +8932,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9">
       <c r="A114" s="1" t="s">
         <v>528</v>
       </c>
@@ -8969,7 +8961,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9">
       <c r="A115" s="1" t="s">
         <v>336</v>
       </c>
@@ -8998,7 +8990,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9">
       <c r="A116" s="1" t="s">
         <v>208</v>
       </c>
@@ -9027,7 +9019,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9">
       <c r="A117" s="1" t="s">
         <v>1006</v>
       </c>
@@ -9056,7 +9048,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9">
       <c r="A118" s="1" t="s">
         <v>51</v>
       </c>
@@ -9085,7 +9077,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9">
       <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
@@ -9114,7 +9106,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9">
       <c r="A120" s="1" t="s">
         <v>523</v>
       </c>
@@ -9143,7 +9135,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9">
       <c r="A121" s="1" t="s">
         <v>1268</v>
       </c>
@@ -9172,7 +9164,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9">
       <c r="A122" s="1" t="s">
         <v>96</v>
       </c>
@@ -9201,7 +9193,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9">
       <c r="A123" s="1" t="s">
         <v>205</v>
       </c>
@@ -9230,7 +9222,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9">
       <c r="A124" s="1" t="s">
         <v>1264</v>
       </c>
@@ -9259,7 +9251,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9">
       <c r="A125" s="1" t="s">
         <v>1677</v>
       </c>
@@ -9288,7 +9280,7 @@
         <v>1681</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9">
       <c r="A126" s="1" t="s">
         <v>10</v>
       </c>
@@ -9314,7 +9306,7 @@
         <v>1676</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9">
       <c r="A127" s="1" t="s">
         <v>36</v>
       </c>
@@ -9343,7 +9335,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9">
       <c r="A128" s="1" t="s">
         <v>32</v>
       </c>
@@ -9372,7 +9364,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9">
       <c r="A129" s="1" t="s">
         <v>103</v>
       </c>
@@ -9401,24 +9393,24 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9">
       <c r="A130" s="1" t="s">
         <v>201</v>
       </c>
       <c r="B130" s="1" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>1742</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>1743</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E130" s="1" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F130" s="1" t="s">
         <v>1744</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>1745</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>63</v>
@@ -9427,10 +9419,10 @@
         <v>12027</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>1746</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
       <c r="A131" s="1" t="s">
         <v>10</v>
       </c>
@@ -9459,7 +9451,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9">
       <c r="A132" s="1" t="s">
         <v>13</v>
       </c>
@@ -9485,7 +9477,7 @@
         <v>7512</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9">
       <c r="A133" s="1" t="s">
         <v>7</v>
       </c>
@@ -9511,7 +9503,7 @@
         <v>7512</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9">
       <c r="A134" s="1" t="s">
         <v>473</v>
       </c>
@@ -9540,7 +9532,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9">
       <c r="A135" s="1" t="s">
         <v>490</v>
       </c>
@@ -9563,7 +9555,7 @@
         <v>8053</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9">
       <c r="A136" s="1" t="s">
         <v>291</v>
       </c>
@@ -9592,7 +9584,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9">
       <c r="A137" s="1" t="s">
         <v>1237</v>
       </c>
@@ -9621,7 +9613,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9">
       <c r="A138" s="1" t="s">
         <v>60</v>
       </c>
@@ -9650,7 +9642,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9">
       <c r="A139" s="1" t="s">
         <v>41</v>
       </c>
@@ -9679,7 +9671,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9">
       <c r="A140" s="1" t="s">
         <v>570</v>
       </c>
@@ -9708,7 +9700,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9">
       <c r="A141" s="1" t="s">
         <v>276</v>
       </c>
@@ -9737,7 +9729,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9">
       <c r="A142" s="1" t="s">
         <v>931</v>
       </c>
@@ -9766,7 +9758,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9">
       <c r="A143" s="1" t="s">
         <v>1229</v>
       </c>
@@ -9795,7 +9787,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9">
       <c r="A144" s="1" t="s">
         <v>248</v>
       </c>
@@ -9824,7 +9816,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9">
       <c r="A145" s="1" t="s">
         <v>654</v>
       </c>
@@ -9853,7 +9845,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9">
       <c r="A146" s="1" t="s">
         <v>659</v>
       </c>
@@ -9876,7 +9868,7 @@
         <v>8080</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9">
       <c r="A147" s="1" t="s">
         <v>657</v>
       </c>
@@ -9905,7 +9897,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9">
       <c r="A148" s="1" t="s">
         <v>134</v>
       </c>
@@ -9928,7 +9920,7 @@
         <v>8080</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9">
       <c r="A149" s="1" t="s">
         <v>1691</v>
       </c>
@@ -9951,7 +9943,7 @@
         <v>8080</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9">
       <c r="A150" s="1" t="s">
         <v>585</v>
       </c>
@@ -9974,7 +9966,7 @@
         <v>8080</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9">
       <c r="A151" s="1" t="s">
         <v>656</v>
       </c>
@@ -9997,7 +9989,7 @@
         <v>8080</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9">
       <c r="A152" s="1" t="s">
         <v>653</v>
       </c>
@@ -10020,7 +10012,7 @@
         <v>8080</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9">
       <c r="A153" s="1" t="s">
         <v>272</v>
       </c>
@@ -10049,7 +10041,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9">
       <c r="A154" s="1" t="s">
         <v>312</v>
       </c>
@@ -10060,7 +10052,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9">
       <c r="A155" s="1" t="s">
         <v>466</v>
       </c>
@@ -10089,7 +10081,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9">
       <c r="A156" s="1" t="s">
         <v>1689</v>
       </c>
@@ -10100,7 +10092,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9">
       <c r="A157" s="1" t="s">
         <v>1109</v>
       </c>
@@ -10117,7 +10109,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:9">
       <c r="A158" s="1" t="s">
         <v>483</v>
       </c>
@@ -10146,7 +10138,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9">
       <c r="A159" s="1" t="s">
         <v>593</v>
       </c>
@@ -10175,7 +10167,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9">
       <c r="A160" s="1" t="s">
         <v>363</v>
       </c>
@@ -10204,7 +10196,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9">
       <c r="A161" s="1" t="s">
         <v>668</v>
       </c>
@@ -10233,7 +10225,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9">
       <c r="A162" s="1" t="s">
         <v>96</v>
       </c>
@@ -10262,7 +10254,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9">
       <c r="A163" s="1" t="s">
         <v>96</v>
       </c>
@@ -10291,7 +10283,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9">
       <c r="A164" s="1" t="s">
         <v>69</v>
       </c>
@@ -10302,7 +10294,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9">
       <c r="A165" s="1" t="s">
         <v>490</v>
       </c>
@@ -10331,7 +10323,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:9">
       <c r="A166" s="1" t="s">
         <v>96</v>
       </c>
@@ -10360,7 +10352,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9">
       <c r="A167" s="1" t="s">
         <v>341</v>
       </c>
@@ -10389,7 +10381,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9">
       <c r="A168" s="1" t="s">
         <v>1707</v>
       </c>
@@ -10400,7 +10392,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9">
       <c r="A169" s="1" t="s">
         <v>1006</v>
       </c>
@@ -10411,7 +10403,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9">
       <c r="A170" s="1" t="s">
         <v>1711</v>
       </c>
@@ -10422,7 +10414,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:9">
       <c r="A171" s="1" t="s">
         <v>1159</v>
       </c>
@@ -10433,10 +10425,10 @@
         <v>1562</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>1755</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
       <c r="A172" s="1" t="s">
         <v>117</v>
       </c>
@@ -10465,7 +10457,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:9">
       <c r="A173" s="1" t="s">
         <v>1565</v>
       </c>
@@ -10494,7 +10486,7 @@
         <v>1572</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:9">
       <c r="A174" s="1" t="s">
         <v>208</v>
       </c>
@@ -10505,7 +10497,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:9">
       <c r="A175" s="1" t="s">
         <v>860</v>
       </c>
@@ -10534,7 +10526,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:9">
       <c r="A176" s="1" t="s">
         <v>341</v>
       </c>
@@ -10563,7 +10555,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:9">
       <c r="A177" s="1" t="s">
         <v>455</v>
       </c>
@@ -10592,7 +10584,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:9">
       <c r="A178" s="1" t="s">
         <v>756</v>
       </c>
@@ -10621,7 +10613,7 @@
         <v>1446</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:9">
       <c r="A179" s="1" t="s">
         <v>208</v>
       </c>
@@ -10650,7 +10642,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:9">
       <c r="A180" s="1" t="s">
         <v>7</v>
       </c>
@@ -10679,7 +10671,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:9">
       <c r="A181" s="1" t="s">
         <v>96</v>
       </c>
@@ -10708,7 +10700,7 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:9">
       <c r="A182" s="1" t="s">
         <v>1518</v>
       </c>
@@ -10734,7 +10726,7 @@
         <v>8543</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9">
       <c r="A183" s="1" t="s">
         <v>466</v>
       </c>
@@ -10763,7 +10755,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:9">
       <c r="A184" s="1" t="s">
         <v>1159</v>
       </c>
@@ -10789,7 +10781,7 @@
         <v>19020</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:9">
       <c r="A185" s="1" t="s">
         <v>96</v>
       </c>
@@ -10818,7 +10810,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:9">
       <c r="A186" s="1" t="s">
         <v>1161</v>
       </c>
@@ -10844,7 +10836,7 @@
         <v>19020</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9">
       <c r="A187" s="1" t="s">
         <v>657</v>
       </c>
@@ -10873,7 +10865,7 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:9">
       <c r="A188" s="1" t="s">
         <v>917</v>
       </c>
@@ -10902,7 +10894,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:9">
       <c r="A189" s="1" t="s">
         <v>372</v>
       </c>
@@ -10931,7 +10923,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:9">
       <c r="A190" s="1" t="s">
         <v>490</v>
       </c>
@@ -10960,7 +10952,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:9">
       <c r="A191" s="1" t="s">
         <v>103</v>
       </c>
@@ -10989,7 +10981,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:9">
       <c r="A192" s="1" t="s">
         <v>368</v>
       </c>
@@ -11018,7 +11010,7 @@
         <v>1615</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:9">
       <c r="A193" s="1" t="s">
         <v>872</v>
       </c>
@@ -11047,7 +11039,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:9">
       <c r="A194" s="1" t="s">
         <v>1159</v>
       </c>
@@ -11073,7 +11065,7 @@
         <v>18070</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:9">
       <c r="A195" s="1" t="s">
         <v>1159</v>
       </c>
@@ -11102,7 +11094,7 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:9">
       <c r="A196" s="1" t="s">
         <v>1046</v>
       </c>
@@ -11116,7 +11108,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:9">
       <c r="A197" s="1" t="s">
         <v>1388</v>
       </c>
@@ -11139,7 +11131,7 @@
         <v>8053</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:9">
       <c r="A198" s="1" t="s">
         <v>1038</v>
       </c>
@@ -11165,7 +11157,7 @@
         <v>8053</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:9">
       <c r="A199" s="1" t="s">
         <v>1036</v>
       </c>
@@ -11191,7 +11183,7 @@
         <v>8053</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:9">
       <c r="A200" s="1" t="s">
         <v>952</v>
       </c>
@@ -11217,7 +11209,7 @@
         <v>8053</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:9">
       <c r="A201" s="1" t="s">
         <v>1390</v>
       </c>
@@ -11240,7 +11232,7 @@
         <v>8053</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:9">
       <c r="A202" s="1" t="s">
         <v>1034</v>
       </c>
@@ -11266,7 +11258,7 @@
         <v>8053</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:9">
       <c r="A203" s="1" t="s">
         <v>103</v>
       </c>
@@ -11295,7 +11287,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:9">
       <c r="A204" s="1" t="s">
         <v>687</v>
       </c>
@@ -11324,7 +11316,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:9">
       <c r="A205" s="1" t="s">
         <v>280</v>
       </c>
@@ -11353,7 +11345,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:9">
       <c r="A206" s="1" t="s">
         <v>558</v>
       </c>
@@ -11382,7 +11374,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:9">
       <c r="A207" s="1" t="s">
         <v>879</v>
       </c>
@@ -11411,7 +11403,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:9">
       <c r="A208" s="1" t="s">
         <v>7</v>
       </c>
@@ -11440,7 +11432,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:9">
       <c r="A209" s="1" t="s">
         <v>32</v>
       </c>
@@ -11469,7 +11461,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:9">
       <c r="A210" s="1" t="s">
         <v>214</v>
       </c>
@@ -11498,7 +11490,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:9">
       <c r="A211" s="1" t="s">
         <v>47</v>
       </c>
@@ -11527,7 +11519,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:9">
       <c r="A212" s="1" t="s">
         <v>1273</v>
       </c>
@@ -11556,7 +11548,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:9">
       <c r="A213" s="1" t="s">
         <v>427</v>
       </c>
@@ -11585,7 +11577,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:9">
       <c r="A214" s="1" t="s">
         <v>1402</v>
       </c>
@@ -11614,7 +11606,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:9">
       <c r="A215" s="1" t="s">
         <v>703</v>
       </c>
@@ -11643,7 +11635,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:9">
       <c r="A216" s="1" t="s">
         <v>285</v>
       </c>
@@ -11672,7 +11664,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:9">
       <c r="A217" s="1" t="s">
         <v>1243</v>
       </c>
@@ -11701,7 +11693,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:9">
       <c r="A218" s="1" t="s">
         <v>117</v>
       </c>
@@ -11727,7 +11719,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:9">
       <c r="A219" s="1" t="s">
         <v>1252</v>
       </c>
@@ -11756,7 +11748,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:9">
       <c r="A220" s="1" t="s">
         <v>1302</v>
       </c>
@@ -11785,7 +11777,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:9">
       <c r="A221" s="1" t="s">
         <v>1182</v>
       </c>
@@ -11814,7 +11806,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:9">
       <c r="A222" s="1" t="s">
         <v>194</v>
       </c>
@@ -11843,7 +11835,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:9">
       <c r="A223" s="1" t="s">
         <v>32</v>
       </c>
@@ -11860,7 +11852,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:9">
       <c r="A224" s="1" t="s">
         <v>1006</v>
       </c>
@@ -11889,7 +11881,7 @@
         <v>1504</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:9">
       <c r="A225" s="1" t="s">
         <v>81</v>
       </c>
@@ -11918,7 +11910,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:9">
       <c r="A226" s="1" t="s">
         <v>79</v>
       </c>
@@ -11947,7 +11939,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:9">
       <c r="A227" s="1" t="s">
         <v>82</v>
       </c>
@@ -11976,7 +11968,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:9">
       <c r="A228" s="1" t="s">
         <v>73</v>
       </c>
@@ -12005,7 +11997,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9">
       <c r="A229" s="1" t="s">
         <v>312</v>
       </c>
@@ -12034,7 +12026,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9">
       <c r="A230" s="1" t="s">
         <v>564</v>
       </c>
@@ -12063,7 +12055,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9">
       <c r="A231" s="1" t="s">
         <v>564</v>
       </c>
@@ -12092,7 +12084,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:9">
       <c r="A232" s="1" t="s">
         <v>128</v>
       </c>
@@ -12121,7 +12113,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:9">
       <c r="A233" s="1" t="s">
         <v>171</v>
       </c>
@@ -12150,7 +12142,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:9">
       <c r="A234" s="1" t="s">
         <v>168</v>
       </c>
@@ -12179,7 +12171,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:9">
       <c r="A235" s="1" t="s">
         <v>69</v>
       </c>
@@ -12208,7 +12200,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:9">
       <c r="A236" s="1" t="s">
         <v>824</v>
       </c>
@@ -12237,7 +12229,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:9">
       <c r="A237" s="1" t="s">
         <v>829</v>
       </c>
@@ -12266,7 +12258,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:9">
       <c r="A238" s="1" t="s">
         <v>833</v>
       </c>
@@ -12295,7 +12287,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:9">
       <c r="A239" s="1" t="s">
         <v>7</v>
       </c>
@@ -12324,7 +12316,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:9">
       <c r="A240" s="1" t="s">
         <v>839</v>
       </c>
@@ -12353,7 +12345,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:9">
       <c r="A241" s="1" t="s">
         <v>843</v>
       </c>
@@ -12382,7 +12374,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:9">
       <c r="A242" s="1" t="s">
         <v>468</v>
       </c>
@@ -12411,9 +12403,9 @@
         <v>472</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:9">
       <c r="A243" s="1" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>414</v>
@@ -12422,10 +12414,10 @@
         <v>71</v>
       </c>
       <c r="D243" s="1" t="s">
+        <v>1746</v>
+      </c>
+      <c r="E243" s="1" t="s">
         <v>1747</v>
-      </c>
-      <c r="E243" s="1" t="s">
-        <v>1748</v>
       </c>
       <c r="F243" s="1" t="s">
         <v>442</v>
@@ -12437,24 +12429,24 @@
         <v>8901</v>
       </c>
       <c r="I243" s="1" t="s">
-        <v>1749</v>
-      </c>
-    </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9">
       <c r="A244" s="1" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B244" s="1" t="s">
         <v>1753</v>
       </c>
-      <c r="B244" s="1" t="s">
-        <v>1754</v>
-      </c>
       <c r="C244" s="1" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="D244" s="1" t="s">
+        <v>1746</v>
+      </c>
+      <c r="E244" s="1" t="s">
         <v>1747</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>1748</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>442</v>
@@ -12466,27 +12458,27 @@
         <v>8901</v>
       </c>
       <c r="I244" s="1" t="s">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9">
       <c r="A245" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B245" s="1" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C245" s="1" t="s">
         <v>1761</v>
       </c>
-      <c r="C245" s="1" t="s">
+      <c r="D245" s="1" t="s">
         <v>1762</v>
       </c>
-      <c r="D245" s="1" t="s">
+      <c r="E245" s="1" t="s">
         <v>1763</v>
       </c>
-      <c r="E245" s="1" t="s">
+      <c r="F245" s="1" t="s">
         <v>1764</v>
-      </c>
-      <c r="F245" s="1" t="s">
-        <v>1765</v>
       </c>
       <c r="G245" s="1" t="s">
         <v>18</v>
@@ -12495,10 +12487,10 @@
         <v>7070</v>
       </c>
       <c r="I245" s="1" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9">
       <c r="A246" s="1" t="s">
         <v>438</v>
       </c>
@@ -12527,7 +12519,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:9">
       <c r="A247" s="1" t="s">
         <v>639</v>
       </c>
@@ -12556,7 +12548,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:9">
       <c r="A248" s="1" t="s">
         <v>1350</v>
       </c>
@@ -12585,7 +12577,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:9">
       <c r="A249" s="1" t="s">
         <v>1510</v>
       </c>
@@ -12614,7 +12606,7 @@
         <v>1513</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:9">
       <c r="A250" s="1" t="s">
         <v>341</v>
       </c>
@@ -12643,7 +12635,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:9">
       <c r="A251" s="1" t="s">
         <v>96</v>
       </c>
@@ -12672,7 +12664,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:9">
       <c r="A252" s="1" t="s">
         <v>448</v>
       </c>
@@ -12701,7 +12693,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:9">
       <c r="A253" s="1" t="s">
         <v>341</v>
       </c>
@@ -12727,7 +12719,7 @@
         <v>1653</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:9">
       <c r="A254" s="1" t="s">
         <v>346</v>
       </c>
@@ -12756,7 +12748,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:9">
       <c r="A255" s="1" t="s">
         <v>764</v>
       </c>
@@ -12785,7 +12777,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:9">
       <c r="A256" s="1" t="s">
         <v>329</v>
       </c>
@@ -12814,7 +12806,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:9">
       <c r="A257" s="1" t="s">
         <v>353</v>
       </c>
@@ -12843,7 +12835,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:9">
       <c r="A258" s="1" t="s">
         <v>368</v>
       </c>
@@ -12872,7 +12864,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:9">
       <c r="A259" s="1" t="s">
         <v>248</v>
       </c>
@@ -12901,7 +12893,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:9">
       <c r="A260" s="1" t="s">
         <v>462</v>
       </c>
@@ -12930,7 +12922,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:9">
       <c r="A261" s="1" t="s">
         <v>341</v>
       </c>
@@ -12959,7 +12951,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:9">
       <c r="A262" s="1" t="s">
         <v>69</v>
       </c>
@@ -12988,7 +12980,7 @@
         <v>1543</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:9">
       <c r="A263" s="1" t="s">
         <v>1524</v>
       </c>
@@ -13011,7 +13003,7 @@
         <v>8816</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:9">
       <c r="A264" s="1" t="s">
         <v>128</v>
       </c>
@@ -13040,7 +13032,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:9">
       <c r="A265" s="1" t="s">
         <v>1522</v>
       </c>
@@ -13066,7 +13058,7 @@
         <v>8816</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:9">
       <c r="A266" s="1" t="s">
         <v>65</v>
       </c>
@@ -13095,7 +13087,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:9">
       <c r="A267" s="1" t="s">
         <v>232</v>
       </c>
@@ -13124,7 +13116,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:9">
       <c r="A268" s="1" t="s">
         <v>252</v>
       </c>
@@ -13153,7 +13145,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:9">
       <c r="A269" s="1" t="s">
         <v>988</v>
       </c>
@@ -13182,7 +13174,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:9">
       <c r="A270" s="1" t="s">
         <v>776</v>
       </c>
@@ -13211,7 +13203,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:9">
       <c r="A271" s="1" t="s">
         <v>796</v>
       </c>
@@ -13240,7 +13232,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:9">
       <c r="A272" s="1" t="s">
         <v>764</v>
       </c>
@@ -13269,7 +13261,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:9">
       <c r="A273" s="1" t="s">
         <v>1573</v>
       </c>
@@ -13298,7 +13290,7 @@
         <v>1579</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:9">
       <c r="A274" s="1" t="s">
         <v>69</v>
       </c>
@@ -13315,7 +13307,7 @@
         <v>1646</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:9">
       <c r="A275" s="1" t="s">
         <v>276</v>
       </c>
@@ -13344,7 +13336,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:9">
       <c r="A276" s="1" t="s">
         <v>1549</v>
       </c>
@@ -13373,7 +13365,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:9">
       <c r="A277" s="1" t="s">
         <v>73</v>
       </c>
@@ -13390,7 +13382,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:9">
       <c r="A278" s="1" t="s">
         <v>73</v>
       </c>
@@ -13419,7 +13411,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:9">
       <c r="A279" s="1" t="s">
         <v>1599</v>
       </c>
@@ -13448,7 +13440,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:9">
       <c r="A280" s="1" t="s">
         <v>96</v>
       </c>
@@ -13477,7 +13469,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:9">
       <c r="A281" s="1" t="s">
         <v>1686</v>
       </c>
@@ -13506,7 +13498,7 @@
         <v>1688</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:9">
       <c r="A282" s="1" t="s">
         <v>1682</v>
       </c>
@@ -13535,7 +13527,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:9">
       <c r="A283" s="1" t="s">
         <v>1537</v>
       </c>
@@ -13564,7 +13556,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:9">
       <c r="A284" s="1" t="s">
         <v>208</v>
       </c>
@@ -13593,7 +13585,7 @@
         <v>1541</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:9">
       <c r="A285" s="1" t="s">
         <v>639</v>
       </c>
@@ -13622,7 +13614,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:9">
       <c r="A286" s="1" t="s">
         <v>770</v>
       </c>
@@ -13651,9 +13643,9 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:9">
       <c r="A287" s="1" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="B287" s="1" t="s">
         <v>1386</v>
@@ -13680,7 +13672,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:9">
       <c r="A288" s="1" t="s">
         <v>41</v>
       </c>
@@ -13709,7 +13701,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:9">
       <c r="A289" s="1" t="s">
         <v>7</v>
       </c>
@@ -13738,7 +13730,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:9">
       <c r="A290" s="1" t="s">
         <v>1392</v>
       </c>
@@ -13767,7 +13759,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:9">
       <c r="A291" s="1" t="s">
         <v>1618</v>
       </c>
@@ -13796,7 +13788,7 @@
         <v>1623</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:9">
       <c r="A292" s="1" t="s">
         <v>1587</v>
       </c>
@@ -13825,7 +13817,7 @@
         <v>1626</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:9">
       <c r="A293" s="1" t="s">
         <v>1701</v>
       </c>
@@ -13839,7 +13831,7 @@
         <v>1624</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:9">
       <c r="A294" s="1" t="s">
         <v>609</v>
       </c>
@@ -13868,7 +13860,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:9">
       <c r="A295" s="1" t="s">
         <v>1030</v>
       </c>
@@ -13894,7 +13886,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:9">
       <c r="A296" s="1" t="s">
         <v>1320</v>
       </c>
@@ -13923,7 +13915,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:9">
       <c r="A297" s="1" t="s">
         <v>603</v>
       </c>
@@ -13952,7 +13944,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:9">
       <c r="A298" s="1" t="s">
         <v>304</v>
       </c>
@@ -13981,7 +13973,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:9">
       <c r="A299" s="1" t="s">
         <v>346</v>
       </c>
@@ -14010,7 +14002,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:9">
       <c r="A300" s="1" t="s">
         <v>208</v>
       </c>
@@ -14039,7 +14031,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:9">
       <c r="A301" s="1" t="s">
         <v>502</v>
       </c>
@@ -14068,7 +14060,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:9">
       <c r="A302" s="1" t="s">
         <v>51</v>
       </c>
@@ -14097,7 +14089,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:9">
       <c r="A303" s="1" t="s">
         <v>770</v>
       </c>
@@ -14126,7 +14118,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:9">
       <c r="A304" s="1" t="s">
         <v>134</v>
       </c>
@@ -14155,7 +14147,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:9">
       <c r="A305" s="1" t="s">
         <v>1545</v>
       </c>
@@ -14184,7 +14176,7 @@
         <v>1546</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:9">
       <c r="A306" s="1" t="s">
         <v>1440</v>
       </c>
@@ -14213,21 +14205,21 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:9">
       <c r="A307" s="1" t="s">
         <v>879</v>
       </c>
       <c r="B307" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="C307" s="1" t="s">
         <v>1756</v>
       </c>
-      <c r="C307" s="1" t="s">
+      <c r="D307" s="1" t="s">
         <v>1757</v>
       </c>
-      <c r="D307" s="1" t="s">
+      <c r="E307" s="1" t="s">
         <v>1758</v>
-      </c>
-      <c r="E307" s="1" t="s">
-        <v>1759</v>
       </c>
       <c r="F307" s="1" t="s">
         <v>643</v>
@@ -14239,10 +14231,10 @@
         <v>7054</v>
       </c>
       <c r="I307" s="1" t="s">
-        <v>1760</v>
-      </c>
-    </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1759</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9">
       <c r="A308" s="1" t="s">
         <v>1408</v>
       </c>
@@ -14271,7 +14263,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:9">
       <c r="A309" s="1" t="s">
         <v>110</v>
       </c>
@@ -14300,7 +14292,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:9">
       <c r="A310" s="1" t="s">
         <v>124</v>
       </c>
@@ -14329,7 +14321,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:9">
       <c r="A311" s="1" t="s">
         <v>47</v>
       </c>
@@ -14355,7 +14347,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:9">
       <c r="A312" s="1" t="s">
         <v>932</v>
       </c>
@@ -14384,7 +14376,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:9">
       <c r="A313" s="1" t="s">
         <v>893</v>
       </c>
@@ -14413,7 +14405,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:9">
       <c r="A314" s="1" t="s">
         <v>1136</v>
       </c>
@@ -14442,7 +14434,7 @@
         <v>1609</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:9">
       <c r="A315" s="1" t="s">
         <v>692</v>
       </c>
@@ -14471,7 +14463,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:9">
       <c r="A316" s="1" t="s">
         <v>668</v>
       </c>
@@ -14500,7 +14492,7 @@
         <v>1617</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:9">
       <c r="A317" s="1" t="s">
         <v>341</v>
       </c>
@@ -14529,7 +14521,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:9">
       <c r="A318" s="1" t="s">
         <v>1669</v>
       </c>
@@ -14558,7 +14550,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:9">
       <c r="A319" s="1" t="s">
         <v>1496</v>
       </c>
@@ -14587,7 +14579,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:9">
       <c r="A320" s="1" t="s">
         <v>1337</v>
       </c>
@@ -14616,7 +14608,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:9">
       <c r="A321" s="1" t="s">
         <v>341</v>
       </c>
@@ -14645,7 +14637,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:9">
       <c r="A322" s="1" t="s">
         <v>163</v>
       </c>
@@ -14662,7 +14654,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:9">
       <c r="A323" s="1" t="s">
         <v>160</v>
       </c>
@@ -14679,7 +14671,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:9">
       <c r="A324" s="1" t="s">
         <v>32</v>
       </c>
@@ -14693,7 +14685,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:9">
       <c r="A325" s="1" t="s">
         <v>157</v>
       </c>
@@ -14710,7 +14702,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:9">
       <c r="A326" s="1" t="s">
         <v>770</v>
       </c>
@@ -14739,7 +14731,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:9">
       <c r="A327" s="1" t="s">
         <v>69</v>
       </c>
@@ -14753,7 +14745,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:9">
       <c r="A328" s="1" t="s">
         <v>1705</v>
       </c>
@@ -14767,7 +14759,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:9">
       <c r="A329" s="1" t="s">
         <v>1714</v>
       </c>
@@ -14796,7 +14788,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:9">
       <c r="A330" s="1" t="s">
         <v>73</v>
       </c>
@@ -14825,7 +14817,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:9">
       <c r="A331" s="1" t="s">
         <v>581</v>
       </c>
@@ -14854,7 +14846,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:9">
       <c r="A332" s="1" t="s">
         <v>584</v>
       </c>
@@ -14883,7 +14875,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:9">
       <c r="A333" s="1" t="s">
         <v>20</v>
       </c>
@@ -14909,7 +14901,7 @@
         <v>77046</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:9">
       <c r="A334" s="1" t="s">
         <v>192</v>
       </c>
@@ -14935,7 +14927,7 @@
         <v>77046</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:9">
       <c r="A335" s="1" t="s">
         <v>324</v>
       </c>
@@ -14958,7 +14950,7 @@
         <v>7924</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:9">
       <c r="A336" s="1" t="s">
         <v>1318</v>
       </c>
@@ -14984,7 +14976,7 @@
         <v>7924</v>
       </c>
     </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:9">
       <c r="A337" s="1" t="s">
         <v>20</v>
       </c>
@@ -15007,7 +14999,7 @@
         <v>7924</v>
       </c>
     </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:9">
       <c r="A338" s="1" t="s">
         <v>269</v>
       </c>
@@ -15036,7 +15028,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:9">
       <c r="A339" s="1" t="s">
         <v>7</v>
       </c>
@@ -15065,7 +15057,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="340" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:9">
       <c r="A340" s="1" t="s">
         <v>401</v>
       </c>
@@ -15088,7 +15080,7 @@
         <v>7924</v>
       </c>
     </row>
-    <row r="341" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:9">
       <c r="A341" s="1" t="s">
         <v>490</v>
       </c>
@@ -15117,7 +15109,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="342" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:9">
       <c r="A342" s="1" t="s">
         <v>962</v>
       </c>
@@ -15146,7 +15138,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="343" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:9">
       <c r="A343" s="1" t="s">
         <v>36</v>
       </c>
@@ -15175,7 +15167,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="344" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:9">
       <c r="A344" s="1" t="s">
         <v>1006</v>
       </c>
@@ -15204,7 +15196,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="345" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:9">
       <c r="A345" s="1" t="s">
         <v>41</v>
       </c>
@@ -15230,7 +15222,7 @@
         <v>8073</v>
       </c>
     </row>
-    <row r="346" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:9">
       <c r="A346" s="1" t="s">
         <v>645</v>
       </c>
@@ -15259,7 +15251,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:9">
       <c r="A347" s="1" t="s">
         <v>1188</v>
       </c>
@@ -15288,7 +15280,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="348" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:9">
       <c r="A348" s="1" t="s">
         <v>466</v>
       </c>
@@ -15317,7 +15309,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="349" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:9">
       <c r="A349" s="1" t="s">
         <v>69</v>
       </c>
@@ -15346,7 +15338,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="350" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:9">
       <c r="A350" s="1" t="s">
         <v>36</v>
       </c>
@@ -15375,7 +15367,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="351" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:9">
       <c r="A351" s="1" t="s">
         <v>223</v>
       </c>
@@ -15404,7 +15396,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="352" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:9">
       <c r="A352" s="1" t="s">
         <v>1509</v>
       </c>
@@ -15415,7 +15407,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="353" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:9">
       <c r="A353" s="1" t="s">
         <v>249</v>
       </c>
@@ -15441,7 +15433,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="354" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:9">
       <c r="A354" s="1" t="s">
         <v>270</v>
       </c>
@@ -15470,7 +15462,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="355" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:9">
       <c r="A355" s="1" t="s">
         <v>1125</v>
       </c>
@@ -15493,7 +15485,7 @@
         <v>8210</v>
       </c>
     </row>
-    <row r="356" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:9">
       <c r="A356" s="1" t="s">
         <v>1088</v>
       </c>
@@ -15522,7 +15514,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="357" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:9">
       <c r="A357" s="1" t="s">
         <v>907</v>
       </c>
@@ -15551,7 +15543,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="358" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:9">
       <c r="A358" s="1" t="s">
         <v>7</v>
       </c>
@@ -15580,7 +15572,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="359" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:9">
       <c r="A359" s="1" t="s">
         <v>1219</v>
       </c>
@@ -15606,7 +15598,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="360" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:9">
       <c r="A360" s="1" t="s">
         <v>973</v>
       </c>
@@ -15632,7 +15624,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="361" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:9">
       <c r="A361" s="1" t="s">
         <v>913</v>
       </c>
@@ -15661,7 +15653,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="362" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:9">
       <c r="A362" s="1" t="s">
         <v>194</v>
       </c>
@@ -15690,7 +15682,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="363" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:9">
       <c r="A363" s="1" t="s">
         <v>654</v>
       </c>
@@ -15716,10 +15708,10 @@
         <v>8054</v>
       </c>
       <c r="I363" s="2" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="364" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="364" spans="1:9">
       <c r="A364" s="1" t="s">
         <v>201</v>
       </c>
@@ -15748,7 +15740,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="365" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:9">
       <c r="A365" s="1" t="s">
         <v>764</v>
       </c>
@@ -15774,10 +15766,10 @@
         <v>8054</v>
       </c>
       <c r="I365" s="2" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="366" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="366" spans="1:9">
       <c r="A366" s="1" t="s">
         <v>205</v>
       </c>
@@ -15806,7 +15798,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="367" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:9">
       <c r="A367" s="1" t="s">
         <v>1220</v>
       </c>
@@ -15832,7 +15824,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="368" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:9">
       <c r="A368" s="1" t="s">
         <v>975</v>
       </c>
@@ -15858,7 +15850,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="369" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:9">
       <c r="A369" s="1" t="s">
         <v>975</v>
       </c>
@@ -15884,7 +15876,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="370" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:9">
       <c r="A370" s="1" t="s">
         <v>219</v>
       </c>
@@ -15913,7 +15905,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="371" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:9">
       <c r="A371" s="1" t="s">
         <v>654</v>
       </c>
@@ -15942,7 +15934,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="372" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:9">
       <c r="A372" s="1" t="s">
         <v>261</v>
       </c>
@@ -15971,7 +15963,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="373" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:9">
       <c r="A373" s="1" t="s">
         <v>134</v>
       </c>
@@ -16000,7 +15992,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="374" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:9">
       <c r="A374" s="1" t="s">
         <v>1222</v>
       </c>
@@ -16029,7 +16021,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="375" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:9">
       <c r="A375" s="1" t="s">
         <v>51</v>
       </c>
@@ -16058,7 +16050,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="376" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:9">
       <c r="A376" s="1" t="s">
         <v>413</v>
       </c>
@@ -16087,7 +16079,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="377" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:9">
       <c r="A377" s="1" t="s">
         <v>124</v>
       </c>
@@ -16116,7 +16108,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="378" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:9">
       <c r="A378" s="1" t="s">
         <v>194</v>
       </c>
@@ -16145,7 +16137,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="379" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:9">
       <c r="A379" s="1" t="s">
         <v>7</v>
       </c>
@@ -16162,7 +16154,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="380" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:9">
       <c r="A380" s="1" t="s">
         <v>1478</v>
       </c>
@@ -16191,7 +16183,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="381" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:9">
       <c r="A381" s="1" t="s">
         <v>1061</v>
       </c>
@@ -16220,7 +16212,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="382" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:9">
       <c r="A382" s="1" t="s">
         <v>32</v>
       </c>
@@ -16249,7 +16241,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="383" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:9">
       <c r="A383" s="1" t="s">
         <v>60</v>
       </c>
@@ -16278,7 +16270,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="384" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:9">
       <c r="A384" s="1" t="s">
         <v>1057</v>
       </c>
@@ -16307,7 +16299,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="385" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:9">
       <c r="A385" s="1" t="s">
         <v>205</v>
       </c>
@@ -16336,7 +16328,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="386" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:9">
       <c r="A386" s="1" t="s">
         <v>1505</v>
       </c>
@@ -16365,7 +16357,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="387" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:9">
       <c r="A387" s="1" t="s">
         <v>824</v>
       </c>
@@ -16394,7 +16386,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="388" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:9">
       <c r="A388" s="1" t="s">
         <v>1054</v>
       </c>
@@ -16423,7 +16415,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="389" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:9">
       <c r="A389" s="1" t="s">
         <v>1165</v>
       </c>
@@ -16452,7 +16444,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="390" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:9">
       <c r="A390" s="1" t="s">
         <v>1043</v>
       </c>
@@ -16466,7 +16458,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="391" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:9">
       <c r="A391" s="1" t="s">
         <v>982</v>
       </c>
@@ -16495,7 +16487,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="392" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:9">
       <c r="A392" s="1" t="s">
         <v>978</v>
       </c>
@@ -16524,7 +16516,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="393" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:9">
       <c r="A393" s="1" t="s">
         <v>1114</v>
       </c>
@@ -16541,7 +16533,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="394" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:9">
       <c r="A394" s="1" t="s">
         <v>1312</v>
       </c>
@@ -16555,10 +16547,10 @@
         <v>1311</v>
       </c>
       <c r="I394" s="1" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="395" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="395" spans="1:9">
       <c r="A395" s="1" t="s">
         <v>1309</v>
       </c>
@@ -16572,10 +16564,10 @@
         <v>1311</v>
       </c>
       <c r="I395" s="1" t="s">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="396" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="396" spans="1:9">
       <c r="A396" s="1" t="s">
         <v>1315</v>
       </c>
@@ -16589,10 +16581,10 @@
         <v>1311</v>
       </c>
       <c r="I396" s="1" t="s">
-        <v>1767</v>
-      </c>
-    </row>
-    <row r="397" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="397" spans="1:9">
       <c r="A397" s="1" t="s">
         <v>69</v>
       </c>
@@ -16621,7 +16613,7 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="398" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:9">
       <c r="A398" s="1" t="s">
         <v>622</v>
       </c>
@@ -16650,7 +16642,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="399" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:9">
       <c r="A399" s="1" t="s">
         <v>629</v>
       </c>
@@ -16661,7 +16653,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="400" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:9">
       <c r="A400" s="1" t="s">
         <v>69</v>
       </c>
@@ -16690,7 +16682,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="401" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:9">
       <c r="A401" s="1" t="s">
         <v>668</v>
       </c>
@@ -16719,7 +16711,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="402" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:9">
       <c r="A402" s="1" t="s">
         <v>117</v>
       </c>
@@ -16748,7 +16740,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="403" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:9">
       <c r="A403" s="1" t="s">
         <v>243</v>
       </c>
@@ -16777,7 +16769,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="404" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:9">
       <c r="A404" s="1" t="s">
         <v>7</v>
       </c>
@@ -16806,7 +16798,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="405" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:9">
       <c r="A405" s="1" t="s">
         <v>924</v>
       </c>
@@ -16835,7 +16827,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="406" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:9">
       <c r="A406" s="1" t="s">
         <v>1482</v>
       </c>
@@ -16858,7 +16850,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="407" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:9">
       <c r="A407" s="1" t="s">
         <v>32</v>
       </c>
@@ -16884,7 +16876,7 @@
         <v>8873</v>
       </c>
     </row>
-    <row r="408" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:9">
       <c r="A408" s="1" t="s">
         <v>82</v>
       </c>
@@ -16913,7 +16905,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="409" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:9">
       <c r="A409" s="1" t="s">
         <v>1118</v>
       </c>
@@ -16942,7 +16934,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="410" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:9">
       <c r="A410" s="1" t="s">
         <v>176</v>
       </c>
@@ -16971,7 +16963,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="411" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:9">
       <c r="A411" s="1" t="s">
         <v>25</v>
       </c>
@@ -17000,7 +16992,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="412" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:9">
       <c r="A412" s="1" t="s">
         <v>312</v>
       </c>
@@ -17029,7 +17021,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="413" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:9">
       <c r="A413" s="1" t="s">
         <v>703</v>
       </c>
@@ -17058,7 +17050,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="414" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:9">
       <c r="A414" s="1" t="s">
         <v>466</v>
       </c>
@@ -17087,7 +17079,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="415" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:9">
       <c r="A415" s="1" t="s">
         <v>41</v>
       </c>
@@ -17116,7 +17108,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="416" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:9">
       <c r="A416" s="1" t="s">
         <v>41</v>
       </c>
@@ -17145,7 +17137,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="417" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:9">
       <c r="A417" s="1" t="s">
         <v>180</v>
       </c>

</xml_diff>